<commit_message>
assignment 2 of math
</commit_message>
<xml_diff>
--- a/src/.vuepress/public/data/unisa/AdvancedAnalytic1/assignment2/MelbourneAirportRain.xlsx
+++ b/src/.vuepress/public/data/unisa/AdvancedAnalytic1/assignment2/MelbourneAirportRain.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\01.workspace\27.blog\myblog\src\.vuepress\public\data\unisa\AdvancedAnalytic1\assignment2\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8DAF7FB-D4A7-45F4-BB3D-85E45EB70518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{55D036A7-507C-4E3D-BE0B-EB5558445C9A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23256" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,7 +41,7 @@
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -158,7 +152,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -185,7 +179,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -218,7 +212,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -250,19 +244,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -282,8 +276,15 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -378,17 +379,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -399,6 +394,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -417,7 +418,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
@@ -457,6 +458,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -465,26 +467,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -594,7 +576,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-1AAD-43C4-98EE-3366BDE9A031}"/>
             </c:ext>
@@ -633,76 +615,76 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>1.3115941549164678</c:v>
+                  <c:v>3.0487044910516921</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3018745365527122</c:v>
+                  <c:v>3.5983046583042775</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0487044910516921</c:v>
+                  <c:v>3.9870835476786897</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.5983046583042775</c:v>
+                  <c:v>4.2448829459534334</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.9870835476786897</c:v>
+                  <c:v>4.3964798146978987</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.2448829459534334</c:v>
+                  <c:v>4.4625431200066075</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.3964798146978987</c:v>
+                  <c:v>4.4603363830140994</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.4625431200066075</c:v>
+                  <c:v>4.4042700171165645</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.4603363830140994</c:v>
+                  <c:v>4.3063511519045008</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.4042700171165645</c:v>
+                  <c:v>4.1765571232943675</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.3063511519045008</c:v>
+                  <c:v>4.0231490562305918</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.1765571232943675</c:v>
+                  <c:v>3.8529368985200163</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.0231490562305918</c:v>
+                  <c:v>3.6715043159943219</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.8529368985200163</c:v>
+                  <c:v>3.4833999763596655</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.6715043159943219</c:v>
+                  <c:v>3.2923004530674254</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.4833999763596655</c:v>
+                  <c:v>3.1011490346819044</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.2923004530674254</c:v>
+                  <c:v>2.912274003582386</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.1011490346819044</c:v>
+                  <c:v>2.7274893787875936</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.912274003582386</c:v>
+                  <c:v>2.5481806579493882</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.7274893787875936</c:v>
+                  <c:v>2.3753777154871769</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.5481806579493882</c:v>
+                  <c:v>2.2098166988609953</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.3753777154871769</c:v>
+                  <c:v>2.0519925000700088</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-1AAD-43C4-98EE-3366BDE9A031}"/>
             </c:ext>
@@ -716,12 +698,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="731645408"/>
-        <c:axId val="1638907632"/>
+        <c:axId val="375273728"/>
+        <c:axId val="375316480"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="731645408"/>
+        <c:axId val="375273728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -760,10 +743,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1638907632"/>
+        <c:crossAx val="375316480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -771,7 +754,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1638907632"/>
+        <c:axId val="375316480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -819,10 +802,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="731645408"/>
+        <c:crossAx val="375273728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -836,6 +819,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -861,20 +845,20 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -898,7 +882,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -910,7 +894,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
@@ -964,6 +948,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -972,26 +957,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1027,39 +992,39 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AK$2:$AK$42</c:f>
+              <c:f>Sheet1!$AK$2:$AK$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="41"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
                 <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -1072,36 +1037,12 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>52</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-4C1A-4827-84CD-B22C13A56D8C}"/>
             </c:ext>
@@ -1135,39 +1076,39 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AN$2:$AN$42</c:f>
+              <c:f>Sheet1!$AN$2:$AN$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="41"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>5.5497089780289874</c:v>
+                  <c:v>3.7764566652249854</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4.928022014683588</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.5497089780289874</c:v>
+                  <c:v>5.3532359224453065</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.3532359224453065</c:v>
+                  <c:v>5.2488155100725837</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>5.7007065074912582</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>5.7426886474605858</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.4542976247912298</c:v>
-                </c:pt>
                 <c:pt idx="6">
+                  <c:v>5.7426886474605858</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>5.7007065074912582</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
+                  <c:v>5.7007065074912582</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5.7426886474605858</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5.7426886474605858</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -1179,34 +1120,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.7007065074912582</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>5.7007065074912582</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="20">
                   <c:v>5.7007065074912582</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-4C1A-4827-84CD-B22C13A56D8C}"/>
             </c:ext>
@@ -1220,12 +1140,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1906804144"/>
-        <c:axId val="590951152"/>
+        <c:axId val="375430528"/>
+        <c:axId val="375432320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1906804144"/>
+        <c:axId val="375430528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1264,10 +1185,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="590951152"/>
+        <c:crossAx val="375432320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1275,7 +1196,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="590951152"/>
+        <c:axId val="375432320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1323,10 +1244,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1906804144"/>
+        <c:crossAx val="375430528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1340,6 +1261,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1365,20 +1287,20 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1402,7 +1324,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1413,1139 +1335,27 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>156210</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:rowOff>67627</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>89535</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:rowOff>153352</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="图表 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE190B5E-8155-ABA4-F198-2BEBE7A50061}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AE190B5E-8155-ABA4-F198-2BEBE7A50061}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2565,23 +1375,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>129539</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:rowOff>73342</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>41</xdr:col>
-      <xdr:colOff>447674</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:rowOff>149542</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="图表 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18E3E855-7F5B-E3A1-3EB7-82EA8F040B19}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{18E3E855-7F5B-E3A1-3EB7-82EA8F040B19}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2645,7 +1455,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -2697,7 +1507,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2891,36 +1701,36 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA6802D6-09D4-4773-944B-EB04DF36FE22}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U29" sqref="U29"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AV17" sqref="AV17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="13" width="0" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="6.85546875" customWidth="1"/>
-    <col min="18" max="18" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="2.42578125" customWidth="1"/>
-    <col min="21" max="21" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="6.88671875" customWidth="1"/>
+    <col min="18" max="18" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="2.44140625" customWidth="1"/>
+    <col min="21" max="21" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="1.85546875" customWidth="1"/>
-    <col min="24" max="24" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="1.88671875" customWidth="1"/>
+    <col min="24" max="24" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="6" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="12" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.85546875" customWidth="1"/>
+    <col min="37" max="37" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40" x14ac:dyDescent="0.25">
@@ -2964,57 +1774,57 @@
         <v>11</v>
       </c>
       <c r="N1" s="2"/>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="9" t="s">
+      <c r="Q1" s="7"/>
+      <c r="R1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
-      <c r="X1" s="9"/>
-      <c r="Y1" s="9"/>
-      <c r="AA1" s="15" t="s">
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="AA1" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="AB1" s="15" t="s">
+      <c r="AB1" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="AD1" s="14" t="s">
+      <c r="AD1" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="AE1" s="14" t="s">
+      <c r="AE1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="AF1" s="15" t="s">
+      <c r="AF1" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="AG1" s="15" t="s">
+      <c r="AG1" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="AH1" s="15" t="s">
+      <c r="AH1" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="AJ1" s="15" t="s">
+      <c r="AJ1" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="AK1" s="14" t="s">
+      <c r="AK1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="AL1" s="14" t="s">
+      <c r="AL1" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="AM1" s="15" t="s">
+      <c r="AM1" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="AN1" s="15" t="s">
+      <c r="AN1" s="13" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3067,62 +1877,62 @@
         <f>(S$15-1)*LN(C2)-C2/$S$16-$S$15*LN($S$16)-$S$17</f>
         <v>-5.4191855077819122</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="S2" s="3"/>
-      <c r="U2" s="3" t="s">
+      <c r="S2" s="17"/>
+      <c r="U2" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="V2" s="3"/>
-      <c r="X2" s="4" t="s">
+      <c r="V2" s="17"/>
+      <c r="X2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Y2" s="5">
+      <c r="Y2" s="4">
         <f>MIN(B2:B53)</f>
         <v>1.6</v>
       </c>
-      <c r="AA2" s="6">
+      <c r="AA2" s="5">
         <v>5</v>
       </c>
-      <c r="AB2" s="6">
-        <v>10</v>
-      </c>
-      <c r="AD2" s="16">
+      <c r="AB2" s="5">
+        <v>15</v>
+      </c>
+      <c r="AD2" s="14">
         <v>5</v>
       </c>
-      <c r="AE2" s="17">
+      <c r="AE2" s="15">
         <v>2</v>
       </c>
-      <c r="AF2" s="6">
-        <f>AD2/2</f>
-        <v>2.5</v>
-      </c>
-      <c r="AG2" s="6">
+      <c r="AF2" s="5">
+        <f>AD2/2+5</f>
+        <v>7.5</v>
+      </c>
+      <c r="AG2" s="5">
         <f>_xlfn.GAMMA.DIST(AF2,$S$3,$S$4,FALSE())</f>
-        <v>5.0445929035248761E-3</v>
-      </c>
-      <c r="AH2" s="6">
+        <v>1.1725786504044969E-2</v>
+      </c>
+      <c r="AH2" s="5">
         <f>AG2*$AE$24*5</f>
-        <v>1.3115941549164678</v>
-      </c>
-      <c r="AJ2" s="16">
-        <v>10</v>
-      </c>
-      <c r="AK2" s="17">
-        <v>12</v>
-      </c>
-      <c r="AL2" s="6">
-        <f>AJ2/2</f>
-        <v>5</v>
-      </c>
-      <c r="AM2" s="6">
+        <v>3.0487044910516921</v>
+      </c>
+      <c r="AJ2" s="14">
+        <v>15</v>
+      </c>
+      <c r="AK2" s="15">
+        <v>17</v>
+      </c>
+      <c r="AL2" s="5">
+        <f>AJ2/2+15</f>
+        <v>22.5</v>
+      </c>
+      <c r="AM2" s="5">
         <f>_xlfn.GAMMA.DIST(AL2,$S$15,$S$16,FALSE())</f>
-        <v>2.134503453088072E-2</v>
-      </c>
-      <c r="AN2" s="6">
-        <f>AM2*$AK$23*5</f>
-        <v>5.5497089780289874</v>
+        <v>1.4524833327788405E-2</v>
+      </c>
+      <c r="AN2" s="5">
+        <f>AM2*$AK$16*5</f>
+        <v>3.7764566652249854</v>
       </c>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.25">
@@ -3175,74 +1985,74 @@
         <f t="shared" ref="P3:P53" si="1">(S$15-1)*LN(C3)-C3/$S$16-$S$15*LN($S$16)-$S$17</f>
         <v>-6.9840560066645834</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="R3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="S3" s="6">
+      <c r="S3" s="5">
         <v>1.9784675092476769</v>
       </c>
-      <c r="U3" s="4" t="s">
+      <c r="U3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="V3" s="6">
+      <c r="V3" s="5">
         <f>V5/V4</f>
         <v>2.4468258204670081</v>
       </c>
-      <c r="X3" s="4" t="s">
+      <c r="X3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="Y3" s="5">
+      <c r="Y3" s="4">
         <f>MAX(B2:B53)</f>
         <v>106.4</v>
       </c>
-      <c r="AA3" s="6">
+      <c r="AA3" s="5">
         <f>AA2+5</f>
         <v>10</v>
       </c>
-      <c r="AB3" s="6">
-        <f>AB2+10</f>
-        <v>20</v>
-      </c>
-      <c r="AD3" s="16">
+      <c r="AB3" s="5">
+        <f>AB2+15</f>
+        <v>30</v>
+      </c>
+      <c r="AD3" s="14">
         <v>10</v>
       </c>
-      <c r="AE3" s="17">
+      <c r="AE3" s="15">
         <v>4</v>
       </c>
-      <c r="AF3" s="6">
-        <f t="shared" ref="AF3:AF23" si="2">AD3/2</f>
-        <v>5</v>
-      </c>
-      <c r="AG3" s="6">
+      <c r="AF3" s="5">
+        <f t="shared" ref="AF3:AF23" si="2">AD3/2+5</f>
+        <v>10</v>
+      </c>
+      <c r="AG3" s="5">
         <f t="shared" ref="AG3:AG23" si="3">_xlfn.GAMMA.DIST(AF3,$S$3,$S$4,FALSE())</f>
-        <v>8.8533636021258157E-3</v>
-      </c>
-      <c r="AH3" s="6">
+        <v>1.3839633301170299E-2</v>
+      </c>
+      <c r="AH3" s="5">
         <f t="shared" ref="AH3:AH23" si="4">AG3*$AE$24*5</f>
-        <v>2.3018745365527122</v>
-      </c>
-      <c r="AJ3" s="16">
-        <v>20</v>
-      </c>
-      <c r="AK3" s="17">
+        <v>3.5983046583042775</v>
+      </c>
+      <c r="AJ3" s="14">
+        <v>30</v>
+      </c>
+      <c r="AK3" s="15">
         <v>11</v>
       </c>
-      <c r="AL3" s="6">
-        <f t="shared" ref="AL3:AL22" si="5">AJ3/2</f>
-        <v>10</v>
-      </c>
-      <c r="AM3" s="6">
-        <f t="shared" ref="AM3:AM22" si="6">_xlfn.GAMMA.DIST(AK3,$S$15,$S$16,FALSE())</f>
+      <c r="AL3" s="5">
+        <f t="shared" ref="AL3:AL15" si="5">AJ3/2+15</f>
+        <v>30</v>
+      </c>
+      <c r="AM3" s="5">
+        <f t="shared" ref="AM3:AM15" si="6">_xlfn.GAMMA.DIST(AK3,$S$15,$S$16,FALSE())</f>
         <v>1.8953930825706108E-2</v>
       </c>
-      <c r="AN3" s="6">
-        <f t="shared" ref="AN3:AN22" si="7">AM3*$AK$23*5</f>
+      <c r="AN3" s="5">
+        <f>AM3*$AK$16*5</f>
         <v>4.928022014683588</v>
       </c>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A53" si="8">A3+1</f>
+        <f t="shared" ref="A4:A53" si="7">A3+1</f>
         <v>1973</v>
       </c>
       <c r="B4" s="1">
@@ -3290,67 +2100,67 @@
         <f t="shared" si="1"/>
         <v>-8.1465384487391255</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="R4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="S4" s="6">
+      <c r="S4" s="5">
         <v>21.599858687941957</v>
       </c>
-      <c r="U4" s="4" t="s">
+      <c r="U4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V4" s="6">
+      <c r="V4" s="5">
         <f>V6^2/V5</f>
         <v>17.465327947397139</v>
       </c>
-      <c r="AA4" s="6">
-        <f t="shared" ref="AA4:AA22" si="9">AA3+5</f>
+      <c r="AA4" s="5">
+        <f t="shared" ref="AA4:AA22" si="8">AA3+5</f>
         <v>15</v>
       </c>
-      <c r="AB4" s="6">
-        <f t="shared" ref="AB4:AB42" si="10">AB3+10</f>
-        <v>30</v>
-      </c>
-      <c r="AD4" s="16">
+      <c r="AB4" s="5">
+        <f t="shared" ref="AB4:AB15" si="9">AB3+15</f>
+        <v>45</v>
+      </c>
+      <c r="AD4" s="14">
         <v>15</v>
       </c>
-      <c r="AE4" s="17">
+      <c r="AE4" s="15">
         <v>3</v>
       </c>
-      <c r="AF4" s="6">
+      <c r="AF4" s="5">
         <f t="shared" si="2"/>
-        <v>7.5</v>
-      </c>
-      <c r="AG4" s="6">
+        <v>12.5</v>
+      </c>
+      <c r="AG4" s="5">
         <f t="shared" si="3"/>
-        <v>1.1725786504044969E-2</v>
-      </c>
-      <c r="AH4" s="6">
+        <v>1.5334936721841115E-2</v>
+      </c>
+      <c r="AH4" s="5">
         <f t="shared" si="4"/>
-        <v>3.0487044910516921</v>
-      </c>
-      <c r="AJ4" s="16">
-        <v>30</v>
-      </c>
-      <c r="AK4" s="17">
-        <v>5</v>
-      </c>
-      <c r="AL4" s="6">
+        <v>3.9870835476786897</v>
+      </c>
+      <c r="AJ4" s="14">
+        <v>45</v>
+      </c>
+      <c r="AK4" s="15">
+        <v>7</v>
+      </c>
+      <c r="AL4" s="5">
         <f t="shared" si="5"/>
-        <v>15</v>
-      </c>
-      <c r="AM4" s="6">
+        <v>37.5</v>
+      </c>
+      <c r="AM4" s="5">
         <f t="shared" si="6"/>
-        <v>2.134503453088072E-2</v>
-      </c>
-      <c r="AN4" s="6">
-        <f t="shared" si="7"/>
-        <v>5.5497089780289874</v>
+        <v>2.0589368932481946E-2</v>
+      </c>
+      <c r="AN4" s="5">
+        <f>AM4*$AK$16*5</f>
+        <v>5.3532359224453065</v>
       </c>
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1974</v>
       </c>
       <c r="B5" s="1">
@@ -3398,68 +2208,68 @@
         <f t="shared" si="1"/>
         <v>-4.301873289209512</v>
       </c>
-      <c r="R5" s="4" t="s">
+      <c r="R5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="S5" s="6">
+      <c r="S5" s="5">
         <f>GAMMALN(S3)</f>
         <v>-8.9534116692711226E-3</v>
       </c>
-      <c r="U5" s="4" t="s">
+      <c r="U5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="V5" s="6">
+      <c r="V5" s="5">
         <f>AVERAGE(B2:B53)</f>
         <v>42.734615384615374</v>
       </c>
-      <c r="AA5" s="6">
+      <c r="AA5" s="5">
+        <f t="shared" si="8"/>
+        <v>20</v>
+      </c>
+      <c r="AB5" s="5">
         <f t="shared" si="9"/>
+        <v>60</v>
+      </c>
+      <c r="AD5" s="14">
         <v>20</v>
       </c>
-      <c r="AB5" s="6">
-        <f t="shared" si="10"/>
-        <v>40</v>
-      </c>
-      <c r="AD5" s="16">
-        <v>20</v>
-      </c>
-      <c r="AE5" s="17">
+      <c r="AE5" s="15">
         <v>2</v>
       </c>
-      <c r="AF5" s="6">
+      <c r="AF5" s="5">
         <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="AG5" s="6">
+        <v>15</v>
+      </c>
+      <c r="AG5" s="5">
         <f t="shared" si="3"/>
-        <v>1.3839633301170299E-2</v>
-      </c>
-      <c r="AH5" s="6">
+        <v>1.6326472869051669E-2</v>
+      </c>
+      <c r="AH5" s="5">
         <f t="shared" si="4"/>
-        <v>3.5983046583042775</v>
-      </c>
-      <c r="AJ5" s="16">
-        <v>40</v>
-      </c>
-      <c r="AK5" s="17">
-        <v>7</v>
-      </c>
-      <c r="AL5" s="6">
+        <v>4.2448829459534334</v>
+      </c>
+      <c r="AJ5" s="14">
+        <v>60</v>
+      </c>
+      <c r="AK5" s="15">
+        <v>8</v>
+      </c>
+      <c r="AL5" s="5">
         <f t="shared" si="5"/>
-        <v>20</v>
-      </c>
-      <c r="AM5" s="6">
+        <v>45</v>
+      </c>
+      <c r="AM5" s="5">
         <f t="shared" si="6"/>
-        <v>2.0589368932481946E-2</v>
-      </c>
-      <c r="AN5" s="6">
-        <f t="shared" si="7"/>
-        <v>5.3532359224453065</v>
+        <v>2.0187751961817633E-2</v>
+      </c>
+      <c r="AN5" s="5">
+        <f>AM5*$AK$16*5</f>
+        <v>5.2488155100725837</v>
       </c>
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1975</v>
       </c>
       <c r="B6" s="1">
@@ -3507,61 +2317,61 @@
         <f t="shared" si="1"/>
         <v>-4.1579924502978667</v>
       </c>
-      <c r="U6" s="4" t="s">
+      <c r="U6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="V6" s="6">
+      <c r="V6" s="5">
         <f>STDEV(B2:B53)</f>
         <v>27.319847591049818</v>
       </c>
-      <c r="AA6" s="6">
+      <c r="AA6" s="5">
+        <f t="shared" si="8"/>
+        <v>25</v>
+      </c>
+      <c r="AB6" s="5">
         <f t="shared" si="9"/>
+        <v>75</v>
+      </c>
+      <c r="AD6" s="14">
         <v>25</v>
       </c>
-      <c r="AB6" s="6">
-        <f t="shared" si="10"/>
-        <v>50</v>
-      </c>
-      <c r="AD6" s="16">
-        <v>25</v>
-      </c>
-      <c r="AE6" s="17">
+      <c r="AE6" s="15">
         <v>5</v>
       </c>
-      <c r="AF6" s="6">
+      <c r="AF6" s="5">
         <f t="shared" si="2"/>
-        <v>12.5</v>
-      </c>
-      <c r="AG6" s="6">
+        <v>17.5</v>
+      </c>
+      <c r="AG6" s="5">
         <f t="shared" si="3"/>
-        <v>1.5334936721841115E-2</v>
-      </c>
-      <c r="AH6" s="6">
+        <v>1.6909537748838074E-2</v>
+      </c>
+      <c r="AH6" s="5">
         <f t="shared" si="4"/>
-        <v>3.9870835476786897</v>
-      </c>
-      <c r="AJ6" s="16">
-        <v>50</v>
-      </c>
-      <c r="AK6" s="17">
-        <v>2</v>
-      </c>
-      <c r="AL6" s="6">
+        <v>4.3964798146978987</v>
+      </c>
+      <c r="AJ6" s="14">
+        <v>75</v>
+      </c>
+      <c r="AK6" s="15">
+        <v>1</v>
+      </c>
+      <c r="AL6" s="5">
         <f t="shared" si="5"/>
-        <v>25</v>
-      </c>
-      <c r="AM6" s="6">
+        <v>52.5</v>
+      </c>
+      <c r="AM6" s="5">
         <f t="shared" si="6"/>
-        <v>2.2087264028694559E-2</v>
-      </c>
-      <c r="AN6" s="6">
+        <v>2.1925794259581761E-2</v>
+      </c>
+      <c r="AN6" s="5">
+        <f>AM6*$AK$16*5</f>
+        <v>5.7007065074912582</v>
+      </c>
+    </row>
+    <row r="7" spans="1:40" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A7">
         <f t="shared" si="7"/>
-        <v>5.7426886474605858</v>
-      </c>
-    </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <f t="shared" si="8"/>
         <v>1976</v>
       </c>
       <c r="B7" s="1">
@@ -3609,61 +2419,61 @@
         <f t="shared" si="1"/>
         <v>-4.3896095574809468</v>
       </c>
-      <c r="R7" s="7" t="s">
+      <c r="R7" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="S7" s="6">
+      <c r="S7" s="5">
         <f>SUM(O2:O53)</f>
         <v>-241.39442776845863</v>
       </c>
-      <c r="AA7" s="6">
+      <c r="AA7" s="5">
+        <f t="shared" si="8"/>
+        <v>30</v>
+      </c>
+      <c r="AB7" s="5">
         <f t="shared" si="9"/>
+        <v>90</v>
+      </c>
+      <c r="AD7" s="14">
         <v>30</v>
       </c>
-      <c r="AB7" s="6">
-        <f t="shared" si="10"/>
+      <c r="AE7" s="15">
+        <v>4</v>
+      </c>
+      <c r="AF7" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="AG7" s="5">
+        <f t="shared" si="3"/>
+        <v>1.7163627384640799E-2</v>
+      </c>
+      <c r="AH7" s="5">
+        <f t="shared" si="4"/>
+        <v>4.4625431200066075</v>
+      </c>
+      <c r="AJ7" s="14">
+        <v>90</v>
+      </c>
+      <c r="AK7" s="15">
+        <v>2</v>
+      </c>
+      <c r="AL7" s="5">
+        <f t="shared" si="5"/>
         <v>60</v>
       </c>
-      <c r="AD7" s="16">
-        <v>30</v>
-      </c>
-      <c r="AE7" s="17">
-        <v>4</v>
-      </c>
-      <c r="AF7" s="6">
-        <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-      <c r="AG7" s="6">
-        <f t="shared" si="3"/>
-        <v>1.6326472869051669E-2</v>
-      </c>
-      <c r="AH7" s="6">
-        <f t="shared" si="4"/>
-        <v>4.2448829459534334</v>
-      </c>
-      <c r="AJ7" s="16">
-        <v>60</v>
-      </c>
-      <c r="AK7" s="17">
-        <v>6</v>
-      </c>
-      <c r="AL7" s="6">
-        <f t="shared" si="5"/>
-        <v>30</v>
-      </c>
-      <c r="AM7" s="6">
+      <c r="AM7" s="5">
         <f t="shared" si="6"/>
-        <v>2.0978067787658577E-2</v>
-      </c>
-      <c r="AN7" s="6">
-        <f t="shared" si="7"/>
-        <v>5.4542976247912298</v>
+        <v>2.2087264028694559E-2</v>
+      </c>
+      <c r="AN7" s="5">
+        <f>AM7*$AK$16*5</f>
+        <v>5.7426886474605858</v>
       </c>
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1977</v>
       </c>
       <c r="B8" s="1">
@@ -3711,61 +2521,61 @@
         <f t="shared" si="1"/>
         <v>-4.9174790338299568</v>
       </c>
-      <c r="U8" s="4" t="s">
+      <c r="U8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="V8" s="6">
+      <c r="V8" s="5">
         <f>COUNT($S$3:$S$4)</f>
         <v>2</v>
       </c>
-      <c r="AA8" s="6">
+      <c r="AA8" s="5">
+        <f t="shared" si="8"/>
+        <v>35</v>
+      </c>
+      <c r="AB8" s="5">
         <f t="shared" si="9"/>
+        <v>105</v>
+      </c>
+      <c r="AD8" s="14">
         <v>35</v>
       </c>
-      <c r="AB8" s="6">
-        <f t="shared" si="10"/>
-        <v>70</v>
-      </c>
-      <c r="AD8" s="16">
-        <v>35</v>
-      </c>
-      <c r="AE8" s="17">
+      <c r="AE8" s="15">
         <v>3</v>
       </c>
-      <c r="AF8" s="6">
+      <c r="AF8" s="5">
         <f t="shared" si="2"/>
-        <v>17.5</v>
-      </c>
-      <c r="AG8" s="6">
+        <v>22.5</v>
+      </c>
+      <c r="AG8" s="5">
         <f t="shared" si="3"/>
-        <v>1.6909537748838074E-2</v>
-      </c>
-      <c r="AH8" s="6">
+        <v>1.7155139934669612E-2</v>
+      </c>
+      <c r="AH8" s="5">
         <f t="shared" si="4"/>
-        <v>4.3964798146978987</v>
-      </c>
-      <c r="AJ8" s="16">
-        <v>70</v>
-      </c>
-      <c r="AK8" s="17">
-        <v>1</v>
-      </c>
-      <c r="AL8" s="6">
+        <v>4.4603363830140994</v>
+      </c>
+      <c r="AJ8" s="14">
+        <v>105</v>
+      </c>
+      <c r="AK8" s="15">
+        <v>2</v>
+      </c>
+      <c r="AL8" s="5">
         <f t="shared" si="5"/>
-        <v>35</v>
-      </c>
-      <c r="AM8" s="6">
+        <v>67.5</v>
+      </c>
+      <c r="AM8" s="5">
         <f t="shared" si="6"/>
-        <v>2.1925794259581761E-2</v>
-      </c>
-      <c r="AN8" s="6">
+        <v>2.2087264028694559E-2</v>
+      </c>
+      <c r="AN8" s="5">
+        <f>AM8*$AK$16*5</f>
+        <v>5.7426886474605858</v>
+      </c>
+    </row>
+    <row r="9" spans="1:40" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A9">
         <f t="shared" si="7"/>
-        <v>5.7007065074912582</v>
-      </c>
-    </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <f t="shared" si="8"/>
         <v>1978</v>
       </c>
       <c r="B9" s="1">
@@ -3813,68 +2623,68 @@
         <f t="shared" si="1"/>
         <v>-4.1722108817935126</v>
       </c>
-      <c r="R9" s="7" t="s">
+      <c r="R9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="S9" s="6">
+      <c r="S9" s="5">
         <f>S3*S4</f>
         <v>42.734618618434318</v>
       </c>
-      <c r="U9" s="4" t="s">
+      <c r="U9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="V9" s="6" t="b">
+      <c r="V9" s="5" t="b">
         <f>AND($S$3&gt;=0.00001, $S$4 &gt;= 0.00001)</f>
         <v>1</v>
       </c>
-      <c r="AA9" s="6">
+      <c r="AA9" s="5">
+        <f t="shared" si="8"/>
+        <v>40</v>
+      </c>
+      <c r="AB9" s="5">
         <f t="shared" si="9"/>
+        <v>120</v>
+      </c>
+      <c r="AD9" s="14">
         <v>40</v>
       </c>
-      <c r="AB9" s="6">
-        <f t="shared" si="10"/>
-        <v>80</v>
-      </c>
-      <c r="AD9" s="16">
-        <v>40</v>
-      </c>
-      <c r="AE9" s="17">
+      <c r="AE9" s="15">
         <v>3</v>
       </c>
-      <c r="AF9" s="6">
+      <c r="AF9" s="5">
         <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="AG9" s="6">
+        <v>25</v>
+      </c>
+      <c r="AG9" s="5">
         <f t="shared" si="3"/>
-        <v>1.7163627384640799E-2</v>
-      </c>
-      <c r="AH9" s="6">
+        <v>1.6939500065832939E-2</v>
+      </c>
+      <c r="AH9" s="5">
         <f t="shared" si="4"/>
-        <v>4.4625431200066075</v>
-      </c>
-      <c r="AJ9" s="16">
-        <v>80</v>
-      </c>
-      <c r="AK9" s="17">
-        <v>0</v>
-      </c>
-      <c r="AL9" s="6">
+        <v>4.4042700171165645</v>
+      </c>
+      <c r="AJ9" s="14">
+        <v>120</v>
+      </c>
+      <c r="AK9" s="15">
+        <v>1</v>
+      </c>
+      <c r="AL9" s="5">
         <f t="shared" si="5"/>
-        <v>40</v>
-      </c>
-      <c r="AM9" s="6">
+        <v>75</v>
+      </c>
+      <c r="AM9" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AN9" s="6">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2.1925794259581761E-2</v>
+      </c>
+      <c r="AN9" s="5">
+        <f>AM9*$AK$16*5</f>
+        <v>5.7007065074912582</v>
       </c>
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1979</v>
       </c>
       <c r="B10" s="1">
@@ -3922,66 +2732,66 @@
         <f t="shared" si="1"/>
         <v>-4.5572522764610746</v>
       </c>
-      <c r="R10" s="4" t="s">
+      <c r="R10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="S10" s="6">
+      <c r="S10" s="5">
         <f>S3*S4^2</f>
         <v>923.06172324127454</v>
       </c>
-      <c r="U10" s="4"/>
-      <c r="V10" s="6">
+      <c r="U10" s="3"/>
+      <c r="V10" s="5">
         <f>{100,100,0.000001,0.05,FALSE,FALSE,FALSE,1,1,1,0.0001,FALSE}</f>
         <v>100</v>
       </c>
-      <c r="AA10" s="6">
+      <c r="AA10" s="5">
+        <f t="shared" si="8"/>
+        <v>45</v>
+      </c>
+      <c r="AB10" s="5">
         <f t="shared" si="9"/>
+        <v>135</v>
+      </c>
+      <c r="AD10" s="14">
         <v>45</v>
       </c>
-      <c r="AB10" s="6">
-        <f t="shared" si="10"/>
-        <v>90</v>
-      </c>
-      <c r="AD10" s="16">
-        <v>45</v>
-      </c>
-      <c r="AE10" s="17">
+      <c r="AE10" s="15">
         <v>6</v>
       </c>
-      <c r="AF10" s="6">
+      <c r="AF10" s="5">
         <f t="shared" si="2"/>
-        <v>22.5</v>
-      </c>
-      <c r="AG10" s="6">
+        <v>27.5</v>
+      </c>
+      <c r="AG10" s="5">
         <f t="shared" si="3"/>
-        <v>1.7155139934669612E-2</v>
-      </c>
-      <c r="AH10" s="6">
+        <v>1.6562889045786542E-2</v>
+      </c>
+      <c r="AH10" s="5">
         <f t="shared" si="4"/>
-        <v>4.4603363830140994</v>
-      </c>
-      <c r="AJ10" s="16">
-        <v>90</v>
-      </c>
-      <c r="AK10" s="17">
-        <v>2</v>
-      </c>
-      <c r="AL10" s="6">
+        <v>4.3063511519045008</v>
+      </c>
+      <c r="AJ10" s="14">
+        <v>135</v>
+      </c>
+      <c r="AK10" s="15">
+        <v>1</v>
+      </c>
+      <c r="AL10" s="5">
         <f t="shared" si="5"/>
-        <v>45</v>
-      </c>
-      <c r="AM10" s="6">
+        <v>82.5</v>
+      </c>
+      <c r="AM10" s="5">
         <f t="shared" si="6"/>
-        <v>2.2087264028694559E-2</v>
-      </c>
-      <c r="AN10" s="6">
+        <v>2.1925794259581761E-2</v>
+      </c>
+      <c r="AN10" s="5">
+        <f>AM10*$AK$16*5</f>
+        <v>5.7007065074912582</v>
+      </c>
+    </row>
+    <row r="11" spans="1:40" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A11">
         <f t="shared" si="7"/>
-        <v>5.7426886474605858</v>
-      </c>
-    </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <f t="shared" si="8"/>
         <v>1980</v>
       </c>
       <c r="B11" s="1">
@@ -4029,68 +2839,68 @@
         <f t="shared" si="1"/>
         <v>-3.9965660457704475</v>
       </c>
-      <c r="R11" s="7" t="s">
+      <c r="R11" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="S11" s="6">
+      <c r="S11" s="5">
         <f>SQRT(S10)</f>
         <v>30.381930867561305</v>
       </c>
-      <c r="U11" s="4" t="s">
+      <c r="U11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="V11" s="6">
+      <c r="V11" s="5">
         <f>MAX($S$7)</f>
         <v>-241.39442776845863</v>
       </c>
-      <c r="AA11" s="6">
+      <c r="AA11" s="5">
+        <f t="shared" si="8"/>
+        <v>50</v>
+      </c>
+      <c r="AB11" s="5">
         <f t="shared" si="9"/>
+        <v>150</v>
+      </c>
+      <c r="AD11" s="14">
         <v>50</v>
       </c>
-      <c r="AB11" s="6">
-        <f t="shared" si="10"/>
-        <v>100</v>
-      </c>
-      <c r="AD11" s="16">
-        <v>50</v>
-      </c>
-      <c r="AE11" s="17">
+      <c r="AE11" s="15">
         <v>2</v>
       </c>
-      <c r="AF11" s="6">
+      <c r="AF11" s="5">
         <f t="shared" si="2"/>
-        <v>25</v>
-      </c>
-      <c r="AG11" s="6">
+        <v>30</v>
+      </c>
+      <c r="AG11" s="5">
         <f t="shared" si="3"/>
-        <v>1.6939500065832939E-2</v>
-      </c>
-      <c r="AH11" s="6">
+        <v>1.6063681243439876E-2</v>
+      </c>
+      <c r="AH11" s="5">
         <f t="shared" si="4"/>
-        <v>4.4042700171165645</v>
-      </c>
-      <c r="AJ11" s="16">
-        <v>100</v>
-      </c>
-      <c r="AK11" s="17">
-        <v>2</v>
-      </c>
-      <c r="AL11" s="6">
+        <v>4.1765571232943675</v>
+      </c>
+      <c r="AJ11" s="14">
+        <v>150</v>
+      </c>
+      <c r="AK11" s="15">
+        <v>0</v>
+      </c>
+      <c r="AL11" s="5">
         <f t="shared" si="5"/>
-        <v>50</v>
-      </c>
-      <c r="AM11" s="6">
+        <v>90</v>
+      </c>
+      <c r="AM11" s="5">
         <f t="shared" si="6"/>
-        <v>2.2087264028694559E-2</v>
-      </c>
-      <c r="AN11" s="6">
-        <f t="shared" si="7"/>
-        <v>5.7426886474605858</v>
+        <v>0</v>
+      </c>
+      <c r="AN11" s="5">
+        <f>AM11*$AK$16*5</f>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1981</v>
       </c>
       <c r="B12" s="1">
@@ -4138,54 +2948,54 @@
         <f t="shared" si="1"/>
         <v>-4.2728314689504137</v>
       </c>
-      <c r="AA12" s="6">
+      <c r="AA12" s="5">
+        <f t="shared" si="8"/>
+        <v>55</v>
+      </c>
+      <c r="AB12" s="5">
         <f t="shared" si="9"/>
+        <v>165</v>
+      </c>
+      <c r="AD12" s="14">
         <v>55</v>
       </c>
-      <c r="AB12" s="6">
-        <f t="shared" si="10"/>
-        <v>110</v>
-      </c>
-      <c r="AD12" s="16">
-        <v>55</v>
-      </c>
-      <c r="AE12" s="17">
+      <c r="AE12" s="15">
         <v>4</v>
       </c>
-      <c r="AF12" s="6">
+      <c r="AF12" s="5">
         <f t="shared" si="2"/>
-        <v>27.5</v>
-      </c>
-      <c r="AG12" s="6">
+        <v>32.5</v>
+      </c>
+      <c r="AG12" s="5">
         <f t="shared" si="3"/>
-        <v>1.6562889045786542E-2</v>
-      </c>
-      <c r="AH12" s="6">
+        <v>1.5473650216271508E-2</v>
+      </c>
+      <c r="AH12" s="5">
         <f t="shared" si="4"/>
-        <v>4.3063511519045008</v>
-      </c>
-      <c r="AJ12" s="16">
-        <v>110</v>
-      </c>
-      <c r="AK12" s="17">
+        <v>4.0231490562305918</v>
+      </c>
+      <c r="AJ12" s="14">
+        <v>165</v>
+      </c>
+      <c r="AK12" s="15">
         <v>0</v>
       </c>
-      <c r="AL12" s="6">
+      <c r="AL12" s="5">
         <f t="shared" si="5"/>
-        <v>55</v>
-      </c>
-      <c r="AM12" s="6">
+        <v>97.5</v>
+      </c>
+      <c r="AM12" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AN12" s="6">
-        <f t="shared" si="7"/>
+      <c r="AN12" s="5">
+        <f>AM12*$AK$16*5</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1982</v>
       </c>
       <c r="B13" s="1">
@@ -4233,64 +3043,64 @@
         <f t="shared" si="1"/>
         <v>-3.8716197758143851</v>
       </c>
-      <c r="R13" s="9" t="s">
+      <c r="R13" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="S13" s="9"/>
-      <c r="T13" s="9"/>
-      <c r="U13" s="9"/>
-      <c r="V13" s="9"/>
-      <c r="W13" s="9"/>
-      <c r="X13" s="9"/>
-      <c r="Y13" s="9"/>
-      <c r="AA13" s="6">
+      <c r="S13" s="16"/>
+      <c r="T13" s="16"/>
+      <c r="U13" s="16"/>
+      <c r="V13" s="16"/>
+      <c r="W13" s="16"/>
+      <c r="X13" s="16"/>
+      <c r="Y13" s="16"/>
+      <c r="AA13" s="5">
+        <f t="shared" si="8"/>
+        <v>60</v>
+      </c>
+      <c r="AB13" s="5">
         <f t="shared" si="9"/>
+        <v>180</v>
+      </c>
+      <c r="AD13" s="14">
         <v>60</v>
       </c>
-      <c r="AB13" s="6">
-        <f t="shared" si="10"/>
-        <v>120</v>
-      </c>
-      <c r="AD13" s="16">
-        <v>60</v>
-      </c>
-      <c r="AE13" s="17">
+      <c r="AE13" s="15">
         <v>3</v>
       </c>
-      <c r="AF13" s="6">
+      <c r="AF13" s="5">
         <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-      <c r="AG13" s="6">
+        <v>35</v>
+      </c>
+      <c r="AG13" s="5">
         <f t="shared" si="3"/>
-        <v>1.6063681243439876E-2</v>
-      </c>
-      <c r="AH13" s="6">
+        <v>1.4818988071230832E-2</v>
+      </c>
+      <c r="AH13" s="5">
         <f t="shared" si="4"/>
-        <v>4.1765571232943675</v>
-      </c>
-      <c r="AJ13" s="16">
-        <v>120</v>
-      </c>
-      <c r="AK13" s="17">
+        <v>3.8529368985200163</v>
+      </c>
+      <c r="AJ13" s="14">
+        <v>180</v>
+      </c>
+      <c r="AK13" s="15">
         <v>1</v>
       </c>
-      <c r="AL13" s="6">
+      <c r="AL13" s="5">
         <f t="shared" si="5"/>
-        <v>60</v>
-      </c>
-      <c r="AM13" s="6">
+        <v>105</v>
+      </c>
+      <c r="AM13" s="5">
         <f t="shared" si="6"/>
         <v>2.1925794259581761E-2</v>
       </c>
-      <c r="AN13" s="6">
-        <f t="shared" si="7"/>
+      <c r="AN13" s="5">
+        <f>AM13*$AK$16*5</f>
         <v>5.7007065074912582</v>
       </c>
     </row>
     <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1983</v>
       </c>
       <c r="B14" s="1">
@@ -4338,69 +3148,69 @@
         <f t="shared" si="1"/>
         <v>-3.9067162391752639</v>
       </c>
-      <c r="R14" s="3" t="s">
+      <c r="R14" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="S14" s="3"/>
-      <c r="U14" s="3" t="s">
+      <c r="S14" s="17"/>
+      <c r="U14" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="V14" s="3"/>
-      <c r="X14" s="4" t="s">
+      <c r="V14" s="17"/>
+      <c r="X14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Y14" s="5">
+      <c r="Y14" s="4">
         <f>MIN($C$2:$C$53)</f>
         <v>1</v>
       </c>
-      <c r="AA14" s="6">
+      <c r="AA14" s="5">
+        <f t="shared" si="8"/>
+        <v>65</v>
+      </c>
+      <c r="AB14" s="5">
         <f t="shared" si="9"/>
+        <v>195</v>
+      </c>
+      <c r="AD14" s="14">
         <v>65</v>
       </c>
-      <c r="AB14" s="6">
-        <f t="shared" si="10"/>
-        <v>130</v>
-      </c>
-      <c r="AD14" s="16">
-        <v>65</v>
-      </c>
-      <c r="AE14" s="17">
+      <c r="AE14" s="15">
         <v>1</v>
       </c>
-      <c r="AF14" s="6">
+      <c r="AF14" s="5">
         <f t="shared" si="2"/>
-        <v>32.5</v>
-      </c>
-      <c r="AG14" s="6">
+        <v>37.5</v>
+      </c>
+      <c r="AG14" s="5">
         <f t="shared" si="3"/>
-        <v>1.5473650216271508E-2</v>
-      </c>
-      <c r="AH14" s="6">
+        <v>1.4121170446132007E-2</v>
+      </c>
+      <c r="AH14" s="5">
         <f t="shared" si="4"/>
-        <v>4.0231490562305918</v>
-      </c>
-      <c r="AJ14" s="16">
-        <v>130</v>
-      </c>
-      <c r="AK14" s="17">
+        <v>3.6715043159943219</v>
+      </c>
+      <c r="AJ14" s="14">
+        <v>195</v>
+      </c>
+      <c r="AK14" s="15">
         <v>0</v>
       </c>
-      <c r="AL14" s="6">
+      <c r="AL14" s="5">
         <f t="shared" si="5"/>
-        <v>65</v>
-      </c>
-      <c r="AM14" s="6">
+        <v>112.5</v>
+      </c>
+      <c r="AM14" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AN14" s="6">
-        <f t="shared" si="7"/>
+      <c r="AN14" s="5">
+        <f>AM14*$AK$16*5</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1984</v>
       </c>
       <c r="B15" s="1">
@@ -4448,74 +3258,74 @@
         <f t="shared" si="1"/>
         <v>-4.1156268609600097</v>
       </c>
-      <c r="R15" s="4" t="s">
+      <c r="R15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="S15" s="6">
+      <c r="S15" s="5">
         <v>1.0483120388058396</v>
       </c>
-      <c r="U15" s="4" t="s">
+      <c r="U15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="V15" s="6">
+      <c r="V15" s="5">
         <f>V17/V16</f>
         <v>0.87181513106797792</v>
       </c>
-      <c r="X15" s="4" t="s">
+      <c r="X15" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="Y15" s="5">
+      <c r="Y15" s="4">
         <f>MAX($C$2:$C$53)</f>
         <v>200.6</v>
       </c>
-      <c r="AA15" s="6">
+      <c r="AA15" s="5">
+        <f t="shared" si="8"/>
+        <v>70</v>
+      </c>
+      <c r="AB15" s="5">
         <f t="shared" si="9"/>
+        <v>210</v>
+      </c>
+      <c r="AD15" s="14">
         <v>70</v>
       </c>
-      <c r="AB15" s="6">
-        <f t="shared" si="10"/>
-        <v>140</v>
-      </c>
-      <c r="AD15" s="16">
-        <v>70</v>
-      </c>
-      <c r="AE15" s="17">
+      <c r="AE15" s="15">
         <v>1</v>
       </c>
-      <c r="AF15" s="6">
+      <c r="AF15" s="5">
         <f t="shared" si="2"/>
-        <v>35</v>
-      </c>
-      <c r="AG15" s="6">
+        <v>40</v>
+      </c>
+      <c r="AG15" s="5">
         <f t="shared" si="3"/>
-        <v>1.4818988071230832E-2</v>
-      </c>
-      <c r="AH15" s="6">
+        <v>1.3397692216767945E-2</v>
+      </c>
+      <c r="AH15" s="5">
         <f t="shared" si="4"/>
-        <v>3.8529368985200163</v>
-      </c>
-      <c r="AJ15" s="16">
-        <v>140</v>
-      </c>
-      <c r="AK15" s="17">
+        <v>3.4833999763596655</v>
+      </c>
+      <c r="AJ15" s="14">
+        <v>210</v>
+      </c>
+      <c r="AK15" s="15">
         <v>1</v>
       </c>
-      <c r="AL15" s="6">
+      <c r="AL15" s="5">
         <f t="shared" si="5"/>
-        <v>70</v>
-      </c>
-      <c r="AM15" s="6">
+        <v>120</v>
+      </c>
+      <c r="AM15" s="5">
         <f t="shared" si="6"/>
         <v>2.1925794259581761E-2</v>
       </c>
-      <c r="AN15" s="6">
+      <c r="AN15" s="5">
+        <f>AM15*$AK$16*5</f>
+        <v>5.7007065074912582</v>
+      </c>
+    </row>
+    <row r="16" spans="1:40" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16">
         <f t="shared" si="7"/>
-        <v>5.7007065074912582</v>
-      </c>
-    </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <f t="shared" si="8"/>
         <v>1985</v>
       </c>
       <c r="B16" s="1">
@@ -4563,67 +3373,52 @@
         <f t="shared" si="1"/>
         <v>-3.8502713010438869</v>
       </c>
-      <c r="R16" s="4" t="s">
+      <c r="R16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="S16" s="6">
+      <c r="S16" s="5">
         <v>38.24097162248173</v>
       </c>
-      <c r="U16" s="4" t="s">
+      <c r="U16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V16" s="6">
+      <c r="V16" s="5">
         <f>V18^2/V17</f>
         <v>45.982754955575246</v>
       </c>
-      <c r="AA16" s="6">
-        <f t="shared" si="9"/>
+      <c r="AA16" s="5">
+        <f t="shared" si="8"/>
         <v>75</v>
       </c>
-      <c r="AB16" s="6">
-        <f t="shared" si="10"/>
-        <v>150</v>
-      </c>
-      <c r="AD16" s="16">
+      <c r="AB16" s="5">
+        <v>15</v>
+      </c>
+      <c r="AD16" s="14">
         <v>75</v>
       </c>
-      <c r="AE16" s="17">
+      <c r="AE16" s="15">
         <v>2</v>
       </c>
-      <c r="AF16" s="6">
+      <c r="AF16" s="5">
         <f t="shared" si="2"/>
-        <v>37.5</v>
-      </c>
-      <c r="AG16" s="6">
+        <v>42.5</v>
+      </c>
+      <c r="AG16" s="5">
         <f t="shared" si="3"/>
-        <v>1.4121170446132007E-2</v>
-      </c>
-      <c r="AH16" s="6">
+        <v>1.2662694050259328E-2</v>
+      </c>
+      <c r="AH16" s="5">
         <f t="shared" si="4"/>
-        <v>3.6715043159943219</v>
-      </c>
-      <c r="AJ16" s="16">
-        <v>150</v>
-      </c>
-      <c r="AK16" s="17">
-        <v>0</v>
-      </c>
-      <c r="AL16" s="6">
-        <f t="shared" si="5"/>
-        <v>75</v>
-      </c>
-      <c r="AM16" s="6">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AN16" s="6">
+        <v>3.2923004530674254</v>
+      </c>
+      <c r="AJ16" s="11"/>
+      <c r="AK16" s="11">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A17">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <f t="shared" si="8"/>
         <v>1986</v>
       </c>
       <c r="B17" s="1">
@@ -4671,68 +3466,51 @@
         <f t="shared" si="1"/>
         <v>-3.9484718907896665</v>
       </c>
-      <c r="R17" s="4" t="s">
+      <c r="R17" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="S17" s="6">
+      <c r="S17" s="5">
         <f>GAMMALN(S15)</f>
         <v>-2.6010544778373997E-2</v>
       </c>
-      <c r="U17" s="4" t="s">
+      <c r="U17" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="V17" s="6">
+      <c r="V17" s="5">
         <f>AVERAGE($C$2:$C$53)</f>
         <v>40.088461538461544</v>
       </c>
-      <c r="AA17" s="6">
-        <f t="shared" si="9"/>
+      <c r="AA17" s="5">
+        <f t="shared" si="8"/>
         <v>80</v>
       </c>
-      <c r="AB17" s="6">
-        <f t="shared" si="10"/>
-        <v>160</v>
-      </c>
-      <c r="AD17" s="16">
+      <c r="AB17" s="5">
+        <v>15</v>
+      </c>
+      <c r="AD17" s="14">
         <v>80</v>
       </c>
-      <c r="AE17" s="17">
+      <c r="AE17" s="15">
         <v>1</v>
       </c>
-      <c r="AF17" s="6">
+      <c r="AF17" s="5">
         <f t="shared" si="2"/>
-        <v>40</v>
-      </c>
-      <c r="AG17" s="6">
+        <v>45</v>
+      </c>
+      <c r="AG17" s="5">
         <f t="shared" si="3"/>
-        <v>1.3397692216767945E-2</v>
-      </c>
-      <c r="AH17" s="6">
+        <v>1.1927496287238094E-2</v>
+      </c>
+      <c r="AH17" s="5">
         <f t="shared" si="4"/>
-        <v>3.4833999763596655</v>
-      </c>
-      <c r="AJ17" s="16">
-        <v>160</v>
-      </c>
-      <c r="AK17" s="17">
-        <v>0</v>
-      </c>
-      <c r="AL17" s="6">
-        <f t="shared" si="5"/>
-        <v>80</v>
-      </c>
-      <c r="AM17" s="6">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AN17" s="6">
+        <v>3.1011490346819044</v>
+      </c>
+      <c r="AJ17" s="9"/>
+      <c r="AK17" s="10"/>
+    </row>
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A18">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <f t="shared" si="8"/>
         <v>1987</v>
       </c>
       <c r="B18" s="1">
@@ -4780,61 +3558,44 @@
         <f t="shared" si="1"/>
         <v>-4.8671432819867073</v>
       </c>
-      <c r="U18" s="4" t="s">
+      <c r="U18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="V18" s="6">
+      <c r="V18" s="5">
         <f>STDEV($C$2:$C$53)</f>
         <v>42.934577015141073</v>
       </c>
-      <c r="AA18" s="6">
-        <f t="shared" si="9"/>
+      <c r="AA18" s="5">
+        <f t="shared" si="8"/>
         <v>85</v>
       </c>
-      <c r="AB18" s="6">
-        <f t="shared" si="10"/>
-        <v>170</v>
-      </c>
-      <c r="AD18" s="16">
+      <c r="AB18" s="5">
+        <v>15</v>
+      </c>
+      <c r="AD18" s="14">
         <v>85</v>
       </c>
-      <c r="AE18" s="17">
+      <c r="AE18" s="15">
         <v>0</v>
       </c>
-      <c r="AF18" s="6">
+      <c r="AF18" s="5">
         <f t="shared" si="2"/>
-        <v>42.5</v>
-      </c>
-      <c r="AG18" s="6">
+        <v>47.5</v>
+      </c>
+      <c r="AG18" s="5">
         <f t="shared" si="3"/>
-        <v>1.2662694050259328E-2</v>
-      </c>
-      <c r="AH18" s="6">
+        <v>1.1201053859932253E-2</v>
+      </c>
+      <c r="AH18" s="5">
         <f t="shared" si="4"/>
-        <v>3.2923004530674254</v>
-      </c>
-      <c r="AJ18" s="16">
-        <v>170</v>
-      </c>
-      <c r="AK18" s="17">
-        <v>0</v>
-      </c>
-      <c r="AL18" s="6">
-        <f t="shared" si="5"/>
-        <v>85</v>
-      </c>
-      <c r="AM18" s="6">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AN18" s="6">
+        <v>2.912274003582386</v>
+      </c>
+      <c r="AJ18" s="9"/>
+      <c r="AK18" s="10"/>
+    </row>
+    <row r="19" spans="1:37" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A19">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <f t="shared" si="8"/>
         <v>1988</v>
       </c>
       <c r="B19" s="1">
@@ -4882,61 +3643,44 @@
         <f t="shared" si="1"/>
         <v>-3.8946972953522359</v>
       </c>
-      <c r="R19" s="7" t="s">
+      <c r="R19" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="S19" s="6">
+      <c r="S19" s="5">
         <f>SUM(P2:P53)</f>
         <v>-243.90005977098127</v>
       </c>
-      <c r="AA19" s="6">
-        <f t="shared" si="9"/>
+      <c r="AA19" s="5">
+        <f t="shared" si="8"/>
         <v>90</v>
       </c>
-      <c r="AB19" s="6">
-        <f t="shared" si="10"/>
-        <v>180</v>
-      </c>
-      <c r="AD19" s="16">
+      <c r="AB19" s="5">
+        <v>15</v>
+      </c>
+      <c r="AD19" s="14">
         <v>90</v>
       </c>
-      <c r="AE19" s="17">
+      <c r="AE19" s="15">
         <v>2</v>
       </c>
-      <c r="AF19" s="6">
+      <c r="AF19" s="5">
         <f t="shared" si="2"/>
-        <v>45</v>
-      </c>
-      <c r="AG19" s="6">
+        <v>50</v>
+      </c>
+      <c r="AG19" s="5">
         <f t="shared" si="3"/>
-        <v>1.1927496287238094E-2</v>
-      </c>
-      <c r="AH19" s="6">
+        <v>1.0490343764567669E-2</v>
+      </c>
+      <c r="AH19" s="5">
         <f t="shared" si="4"/>
-        <v>3.1011490346819044</v>
-      </c>
-      <c r="AJ19" s="16">
-        <v>180</v>
-      </c>
-      <c r="AK19" s="17">
-        <v>1</v>
-      </c>
-      <c r="AL19" s="6">
-        <f t="shared" si="5"/>
-        <v>90</v>
-      </c>
-      <c r="AM19" s="6">
-        <f t="shared" si="6"/>
-        <v>2.1925794259581761E-2</v>
-      </c>
-      <c r="AN19" s="6">
+        <v>2.7274893787875936</v>
+      </c>
+      <c r="AJ19" s="9"/>
+      <c r="AK19" s="10"/>
+    </row>
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A20">
         <f t="shared" si="7"/>
-        <v>5.7007065074912582</v>
-      </c>
-    </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <f t="shared" si="8"/>
         <v>1989</v>
       </c>
       <c r="B20" s="1">
@@ -4984,61 +3728,44 @@
         <f t="shared" si="1"/>
         <v>-4.0783915489729283</v>
       </c>
-      <c r="U20" s="4" t="s">
+      <c r="U20" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="V20" s="6">
+      <c r="V20" s="5">
         <f>COUNT($S$3:$S$4)</f>
         <v>2</v>
       </c>
-      <c r="AA20" s="6">
-        <f t="shared" si="9"/>
+      <c r="AA20" s="5">
+        <f t="shared" si="8"/>
         <v>95</v>
       </c>
-      <c r="AB20" s="6">
-        <f t="shared" si="10"/>
-        <v>190</v>
-      </c>
-      <c r="AD20" s="16">
+      <c r="AB20" s="5">
+        <v>15</v>
+      </c>
+      <c r="AD20" s="14">
         <v>95</v>
       </c>
-      <c r="AE20" s="17">
+      <c r="AE20" s="15">
         <v>0</v>
       </c>
-      <c r="AF20" s="6">
+      <c r="AF20" s="5">
         <f t="shared" si="2"/>
-        <v>47.5</v>
-      </c>
-      <c r="AG20" s="6">
+        <v>52.5</v>
+      </c>
+      <c r="AG20" s="5">
         <f t="shared" si="3"/>
-        <v>1.1201053859932253E-2</v>
-      </c>
-      <c r="AH20" s="6">
+        <v>9.8006948382668782E-3</v>
+      </c>
+      <c r="AH20" s="5">
         <f t="shared" si="4"/>
-        <v>2.912274003582386</v>
-      </c>
-      <c r="AJ20" s="16">
-        <v>190</v>
-      </c>
-      <c r="AK20" s="17">
-        <v>0</v>
-      </c>
-      <c r="AL20" s="6">
-        <f t="shared" si="5"/>
-        <v>95</v>
-      </c>
-      <c r="AM20" s="6">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AN20" s="6">
+        <v>2.5481806579493882</v>
+      </c>
+      <c r="AJ20" s="9"/>
+      <c r="AK20" s="10"/>
+    </row>
+    <row r="21" spans="1:37" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A21">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <f t="shared" si="8"/>
         <v>1990</v>
       </c>
       <c r="B21" s="1">
@@ -5086,68 +3813,52 @@
         <f t="shared" si="1"/>
         <v>-6.6851958352646212</v>
       </c>
-      <c r="R21" s="7" t="s">
+      <c r="R21" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="S21" s="6">
+      <c r="S21" s="5">
         <f>S15*S16</f>
         <v>40.088470927480074</v>
       </c>
-      <c r="U21" s="4" t="s">
+      <c r="U21" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="V21" s="6" t="b">
+      <c r="V21" s="5" t="b">
         <f>AND($S$15&gt;=0.00001, $S$16 &gt;= 0.00001)</f>
         <v>1</v>
       </c>
-      <c r="AA21" s="6">
-        <f t="shared" si="9"/>
+      <c r="AA21" s="5">
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
-      <c r="AB21" s="6">
-        <f t="shared" si="10"/>
-        <v>200</v>
-      </c>
-      <c r="AD21" s="16">
+      <c r="AB21" s="5">
+        <f t="shared" ref="AB4:AB22" si="10">AB20+10</f>
+        <v>25</v>
+      </c>
+      <c r="AD21" s="14">
         <v>100</v>
       </c>
-      <c r="AE21" s="17">
+      <c r="AE21" s="15">
         <v>2</v>
       </c>
-      <c r="AF21" s="6">
+      <c r="AF21" s="5">
         <f t="shared" si="2"/>
-        <v>50</v>
-      </c>
-      <c r="AG21" s="6">
+        <v>55</v>
+      </c>
+      <c r="AG21" s="5">
         <f t="shared" si="3"/>
-        <v>1.0490343764567669E-2</v>
-      </c>
-      <c r="AH21" s="6">
+        <v>9.1360681364891418E-3</v>
+      </c>
+      <c r="AH21" s="5">
         <f t="shared" si="4"/>
-        <v>2.7274893787875936</v>
-      </c>
-      <c r="AJ21" s="16">
-        <v>200</v>
-      </c>
-      <c r="AK21" s="17">
-        <v>0</v>
-      </c>
-      <c r="AL21" s="6">
-        <f t="shared" si="5"/>
-        <v>100</v>
-      </c>
-      <c r="AM21" s="6">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AN21" s="6">
+        <v>2.3753777154871769</v>
+      </c>
+      <c r="AJ21" s="9"/>
+      <c r="AK21" s="10"/>
+    </row>
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A22">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <f t="shared" si="8"/>
         <v>1991</v>
       </c>
       <c r="B22" s="1">
@@ -5195,66 +3906,50 @@
         <f t="shared" si="1"/>
         <v>-3.8200915151733499</v>
       </c>
-      <c r="R22" s="4" t="s">
+      <c r="R22" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="S22" s="6">
+      <c r="S22" s="5">
         <f>S15*S16^2</f>
         <v>1533.0220791264494</v>
       </c>
-      <c r="U22" s="4"/>
-      <c r="V22" s="6">
+      <c r="U22" s="3"/>
+      <c r="V22" s="5">
         <f>{100,100,0.000001,0.05,FALSE,FALSE,FALSE,1,1,1,0.0001,FALSE}</f>
         <v>100</v>
       </c>
-      <c r="AA22" s="6">
-        <f t="shared" si="9"/>
+      <c r="AA22" s="5">
+        <f t="shared" si="8"/>
         <v>105</v>
       </c>
-      <c r="AB22" s="6">
+      <c r="AB22" s="5">
         <f t="shared" si="10"/>
-        <v>210</v>
-      </c>
-      <c r="AD22" s="16">
+        <v>35</v>
+      </c>
+      <c r="AD22" s="14">
         <v>105</v>
       </c>
-      <c r="AE22" s="17">
+      <c r="AE22" s="15">
         <v>1</v>
       </c>
-      <c r="AF22" s="6">
+      <c r="AF22" s="5">
         <f t="shared" si="2"/>
-        <v>52.5</v>
-      </c>
-      <c r="AG22" s="6">
+        <v>57.5</v>
+      </c>
+      <c r="AG22" s="5">
         <f t="shared" si="3"/>
-        <v>9.8006948382668782E-3</v>
-      </c>
-      <c r="AH22" s="6">
+        <v>8.4992949956192131E-3</v>
+      </c>
+      <c r="AH22" s="5">
         <f t="shared" si="4"/>
-        <v>2.5481806579493882</v>
-      </c>
-      <c r="AJ22" s="16">
-        <v>210</v>
-      </c>
-      <c r="AK22" s="17">
-        <v>1</v>
-      </c>
-      <c r="AL22" s="6">
-        <f t="shared" si="5"/>
-        <v>105</v>
-      </c>
-      <c r="AM22" s="6">
-        <f t="shared" si="6"/>
-        <v>2.1925794259581761E-2</v>
-      </c>
-      <c r="AN22" s="6">
+        <v>2.2098166988609953</v>
+      </c>
+      <c r="AJ22" s="9"/>
+      <c r="AK22" s="10"/>
+    </row>
+    <row r="23" spans="1:37" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A23">
         <f t="shared" si="7"/>
-        <v>5.7007065074912582</v>
-      </c>
-    </row>
-    <row r="23" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <f t="shared" si="8"/>
         <v>1992</v>
       </c>
       <c r="B23" s="1">
@@ -5302,51 +3997,49 @@
         <f t="shared" si="1"/>
         <v>-4.1912360197238483</v>
       </c>
-      <c r="R23" s="7" t="s">
+      <c r="R23" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="S23" s="6">
+      <c r="S23" s="5">
         <f>SQRT(S22)</f>
         <v>39.153825855546344</v>
       </c>
-      <c r="U23" s="4" t="s">
+      <c r="U23" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="V23" s="6">
+      <c r="V23" s="5">
         <f>MAX($S$7)</f>
         <v>-241.39442776845863</v>
       </c>
-      <c r="AA23" s="6">
+      <c r="AA23" s="5">
         <f>AA22+5</f>
         <v>110</v>
       </c>
-      <c r="AB23" s="6"/>
-      <c r="AD23" s="16">
+      <c r="AB23" s="5"/>
+      <c r="AD23" s="14">
         <v>110</v>
       </c>
-      <c r="AE23" s="17">
+      <c r="AE23" s="15">
         <v>1</v>
       </c>
-      <c r="AF23" s="6">
+      <c r="AF23" s="5">
         <f t="shared" si="2"/>
-        <v>55</v>
-      </c>
-      <c r="AG23" s="6">
+        <v>60</v>
+      </c>
+      <c r="AG23" s="5">
         <f t="shared" si="3"/>
-        <v>9.1360681364891418E-3</v>
-      </c>
-      <c r="AH23" s="6">
+        <v>7.8922788464231113E-3</v>
+      </c>
+      <c r="AH23" s="5">
         <f t="shared" si="4"/>
-        <v>2.3753777154871769</v>
-      </c>
-      <c r="AJ23" s="13"/>
-      <c r="AK23" s="13">
-        <v>52</v>
-      </c>
+        <v>2.0519925000700088</v>
+      </c>
+      <c r="AJ23" s="9"/>
+      <c r="AK23" s="10"/>
     </row>
-    <row r="24" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:37" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1993</v>
       </c>
       <c r="B24" s="1">
@@ -5394,17 +4087,17 @@
         <f t="shared" si="1"/>
         <v>-4.6617227919628883</v>
       </c>
-      <c r="AD24" s="13"/>
-      <c r="AE24" s="13">
+      <c r="AD24" s="11"/>
+      <c r="AE24" s="11">
         <f>SUM(AE2:AE23)</f>
         <v>52</v>
       </c>
-      <c r="AJ24" s="11"/>
-      <c r="AK24" s="12"/>
+      <c r="AJ24" s="9"/>
+      <c r="AK24" s="10"/>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1994</v>
       </c>
       <c r="B25" s="1">
@@ -5452,12 +4145,12 @@
         <f t="shared" si="1"/>
         <v>-6.0427970956437731</v>
       </c>
-      <c r="AJ25" s="11"/>
-      <c r="AK25" s="12"/>
+      <c r="AJ25" s="9"/>
+      <c r="AK25" s="10"/>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1995</v>
       </c>
       <c r="B26" s="1">
@@ -5505,12 +4198,12 @@
         <f t="shared" si="1"/>
         <v>-4.3115783835177197</v>
       </c>
-      <c r="AJ26" s="11"/>
-      <c r="AK26" s="12"/>
+      <c r="AJ26" s="9"/>
+      <c r="AK26" s="10"/>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1996</v>
       </c>
       <c r="B27" s="1">
@@ -5558,12 +4251,12 @@
         <f t="shared" si="1"/>
         <v>-6.1146048491348859</v>
       </c>
-      <c r="AJ27" s="11"/>
-      <c r="AK27" s="12"/>
+      <c r="AJ27" s="9"/>
+      <c r="AK27" s="10"/>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1997</v>
       </c>
       <c r="B28" s="1">
@@ -5611,12 +4304,12 @@
         <f t="shared" si="1"/>
         <v>-3.8374220539186181</v>
       </c>
-      <c r="AJ28" s="11"/>
-      <c r="AK28" s="12"/>
+      <c r="AJ28" s="9"/>
+      <c r="AK28" s="10"/>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1998</v>
       </c>
       <c r="B29" s="1">
@@ -5664,12 +4357,12 @@
         <f t="shared" si="1"/>
         <v>-5.0082728848241898</v>
       </c>
-      <c r="AJ29" s="11"/>
-      <c r="AK29" s="12"/>
+      <c r="AJ29" s="9"/>
+      <c r="AK29" s="10"/>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1999</v>
       </c>
       <c r="B30" s="1">
@@ -5717,12 +4410,12 @@
         <f t="shared" si="1"/>
         <v>-4.796814711603691</v>
       </c>
-      <c r="AJ30" s="11"/>
-      <c r="AK30" s="12"/>
+      <c r="AJ30" s="9"/>
+      <c r="AK30" s="10"/>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2000</v>
       </c>
       <c r="B31" s="1">
@@ -5770,12 +4463,12 @@
         <f t="shared" si="1"/>
         <v>-4.527519481503246</v>
       </c>
-      <c r="AJ31" s="11"/>
-      <c r="AK31" s="12"/>
+      <c r="AJ31" s="9"/>
+      <c r="AK31" s="10"/>
     </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2001</v>
       </c>
       <c r="B32" s="1">
@@ -5823,12 +4516,12 @@
         <f t="shared" si="1"/>
         <v>-3.9744783094093021</v>
       </c>
-      <c r="AJ32" s="11"/>
-      <c r="AK32" s="12"/>
+      <c r="AJ32" s="9"/>
+      <c r="AK32" s="10"/>
     </row>
     <row r="33" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2002</v>
       </c>
       <c r="B33" s="1">
@@ -5876,12 +4569,12 @@
         <f t="shared" si="1"/>
         <v>-4.9628469976295175</v>
       </c>
-      <c r="AJ33" s="11"/>
-      <c r="AK33" s="12"/>
+      <c r="AJ33" s="9"/>
+      <c r="AK33" s="10"/>
     </row>
     <row r="34" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2003</v>
       </c>
       <c r="B34" s="1">
@@ -5929,12 +4622,12 @@
         <f t="shared" si="1"/>
         <v>-4.120310949044641</v>
       </c>
-      <c r="AJ34" s="11"/>
-      <c r="AK34" s="12"/>
+      <c r="AJ34" s="9"/>
+      <c r="AK34" s="10"/>
     </row>
     <row r="35" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2004</v>
       </c>
       <c r="B35" s="1">
@@ -5982,12 +4675,12 @@
         <f t="shared" si="1"/>
         <v>-3.9399446447948692</v>
       </c>
-      <c r="AJ35" s="11"/>
-      <c r="AK35" s="12"/>
+      <c r="AJ35" s="9"/>
+      <c r="AK35" s="10"/>
     </row>
-    <row r="36" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:38" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2005</v>
       </c>
       <c r="B36" s="1">
@@ -6036,11 +4729,12 @@
         <v>-8.7835069330833218</v>
       </c>
       <c r="AJ36" s="11"/>
-      <c r="AK36" s="12"/>
+      <c r="AK36" s="11"/>
+      <c r="AL36" s="10"/>
     </row>
     <row r="37" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2006</v>
       </c>
       <c r="B37" s="1">
@@ -6088,12 +4782,10 @@
         <f t="shared" si="1"/>
         <v>-5.1347292877409219</v>
       </c>
-      <c r="AJ37" s="11"/>
-      <c r="AK37" s="12"/>
     </row>
     <row r="38" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2007</v>
       </c>
       <c r="B38" s="1">
@@ -6141,12 +4833,10 @@
         <f t="shared" si="1"/>
         <v>-4.0099731404735026</v>
       </c>
-      <c r="AJ38" s="11"/>
-      <c r="AK38" s="12"/>
     </row>
     <row r="39" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A39">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2008</v>
       </c>
       <c r="B39" s="1">
@@ -6194,12 +4884,10 @@
         <f t="shared" si="1"/>
         <v>-4.4436067907869807</v>
       </c>
-      <c r="AJ39" s="11"/>
-      <c r="AK39" s="12"/>
     </row>
     <row r="40" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2009</v>
       </c>
       <c r="B40" s="1">
@@ -6247,12 +4935,10 @@
         <f t="shared" si="1"/>
         <v>-3.8642777780789603</v>
       </c>
-      <c r="AJ40" s="11"/>
-      <c r="AK40" s="12"/>
     </row>
     <row r="41" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A41">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2010</v>
       </c>
       <c r="B41" s="1">
@@ -6300,12 +4986,10 @@
         <f t="shared" si="1"/>
         <v>-4.577104534185346</v>
       </c>
-      <c r="AJ41" s="11"/>
-      <c r="AK41" s="12"/>
     </row>
     <row r="42" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2011</v>
       </c>
       <c r="B42" s="1">
@@ -6353,12 +5037,10 @@
         <f t="shared" si="1"/>
         <v>-5.8634695925845906</v>
       </c>
-      <c r="AJ42" s="11"/>
-      <c r="AK42" s="12"/>
     </row>
-    <row r="43" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A43">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2012</v>
       </c>
       <c r="B43" s="1">
@@ -6406,13 +5088,10 @@
         <f t="shared" si="1"/>
         <v>-5.7151172015810001</v>
       </c>
-      <c r="AJ43" s="13"/>
-      <c r="AK43" s="13"/>
-      <c r="AL43" s="12"/>
     </row>
     <row r="44" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A44">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2013</v>
       </c>
       <c r="B44" s="1">
@@ -6463,7 +5142,7 @@
     </row>
     <row r="45" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A45">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2014</v>
       </c>
       <c r="B45" s="1">
@@ -6514,7 +5193,7 @@
     </row>
     <row r="46" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2015</v>
       </c>
       <c r="B46" s="1">
@@ -6565,7 +5244,7 @@
     </row>
     <row r="47" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A47">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2016</v>
       </c>
       <c r="B47" s="1">
@@ -6616,7 +5295,7 @@
     </row>
     <row r="48" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A48">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2017</v>
       </c>
       <c r="B48" s="1">
@@ -6667,7 +5346,7 @@
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2018</v>
       </c>
       <c r="B49" s="1">
@@ -6718,7 +5397,7 @@
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2019</v>
       </c>
       <c r="B50" s="1">
@@ -6769,7 +5448,7 @@
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2020</v>
       </c>
       <c r="B51" s="1">
@@ -6820,7 +5499,7 @@
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2021</v>
       </c>
       <c r="B52" s="1">
@@ -6871,7 +5550,7 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2022</v>
       </c>
       <c r="B53" s="1">
@@ -6921,17 +5600,18 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="AJ2:AJ22">
+  <sortState ref="AJ2:AJ15">
     <sortCondition ref="AJ2"/>
   </sortState>
   <mergeCells count="6">
+    <mergeCell ref="R1:Y1"/>
     <mergeCell ref="R13:Y13"/>
     <mergeCell ref="R14:S14"/>
     <mergeCell ref="U14:V14"/>
     <mergeCell ref="R2:S2"/>
     <mergeCell ref="U2:V2"/>
-    <mergeCell ref="R1:Y1"/>
   </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
correct the assignment2 of math
</commit_message>
<xml_diff>
--- a/src/.vuepress/public/data/unisa/AdvancedAnalytic1/assignment2/MelbourneAirportRain.xlsx
+++ b/src/.vuepress/public/data/unisa/AdvancedAnalytic1/assignment2/MelbourneAirportRain.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\01.workspace\27.blog\myblog\src\.vuepress\public\data\unisa\AdvancedAnalytic1\assignment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1247D65C-ABB9-4E0A-BFCA-35E106418DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAB54772-8ED3-432E-9A9E-E7C6259B4739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gamma" sheetId="1" r:id="rId1"/>
@@ -510,13 +510,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -7700,7 +7700,7 @@
   <dimension ref="A1:BO1002"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AZ34" sqref="AZ34"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7740,63 +7740,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:67">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
       <c r="O1" s="21" t="s">
         <v>51</v>
       </c>
       <c r="P1" s="21"/>
       <c r="Q1" s="21"/>
-      <c r="S1" s="22" t="s">
+      <c r="S1" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="T1" s="22"/>
-      <c r="U1" s="22"/>
-      <c r="V1" s="22"/>
-      <c r="W1" s="22"/>
-      <c r="X1" s="22"/>
-      <c r="Y1" s="22"/>
-      <c r="Z1" s="22"/>
-      <c r="AA1" s="22"/>
-      <c r="AB1" s="22"/>
-      <c r="AC1" s="22"/>
-      <c r="AD1" s="22"/>
-      <c r="AE1" s="22"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="24"/>
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="24"/>
+      <c r="AA1" s="24"/>
+      <c r="AB1" s="24"/>
+      <c r="AC1" s="24"/>
+      <c r="AD1" s="24"/>
+      <c r="AE1" s="24"/>
       <c r="AG1" s="21" t="s">
         <v>45</v>
       </c>
       <c r="AH1" s="21"/>
       <c r="AI1" s="21"/>
-      <c r="AK1" s="22" t="s">
+      <c r="AK1" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="AL1" s="22"/>
-      <c r="AM1" s="22"/>
-      <c r="AN1" s="22"/>
-      <c r="AO1" s="22"/>
-      <c r="AP1" s="22"/>
-      <c r="AQ1" s="22"/>
-      <c r="AR1" s="22"/>
-      <c r="AS1" s="22"/>
-      <c r="AT1" s="22"/>
-      <c r="AU1" s="22"/>
-      <c r="AV1" s="22"/>
-      <c r="AW1" s="22"/>
-      <c r="AX1" s="22"/>
-      <c r="AY1" s="22"/>
+      <c r="AL1" s="24"/>
+      <c r="AM1" s="24"/>
+      <c r="AN1" s="24"/>
+      <c r="AO1" s="24"/>
+      <c r="AP1" s="24"/>
+      <c r="AQ1" s="24"/>
+      <c r="AR1" s="24"/>
+      <c r="AS1" s="24"/>
+      <c r="AT1" s="24"/>
+      <c r="AU1" s="24"/>
+      <c r="AV1" s="24"/>
+      <c r="AW1" s="24"/>
+      <c r="AX1" s="24"/>
+      <c r="AY1" s="24"/>
       <c r="BA1" s="21" t="s">
         <v>47</v>
       </c>
@@ -7920,56 +7920,56 @@
       <c r="AI2" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="AK2" s="23" t="s">
+      <c r="AK2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="AL2" s="23"/>
-      <c r="AM2" s="23"/>
-      <c r="AN2" s="23" t="s">
+      <c r="AL2" s="22"/>
+      <c r="AM2" s="22"/>
+      <c r="AN2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="AO2" s="23"/>
-      <c r="AP2" s="23"/>
-      <c r="AQ2" s="23" t="s">
+      <c r="AO2" s="22"/>
+      <c r="AP2" s="22"/>
+      <c r="AQ2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="AR2" s="23"/>
-      <c r="AS2" s="23"/>
-      <c r="AT2" s="24" t="s">
+      <c r="AR2" s="22"/>
+      <c r="AS2" s="22"/>
+      <c r="AT2" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="AU2" s="24"/>
-      <c r="AV2" s="24"/>
-      <c r="AW2" s="24" t="s">
+      <c r="AU2" s="23"/>
+      <c r="AV2" s="23"/>
+      <c r="AW2" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="AX2" s="24"/>
-      <c r="AY2" s="24"/>
-      <c r="BA2" s="23" t="s">
+      <c r="AX2" s="23"/>
+      <c r="AY2" s="23"/>
+      <c r="BA2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="BB2" s="23"/>
-      <c r="BC2" s="23"/>
-      <c r="BD2" s="23" t="s">
+      <c r="BB2" s="22"/>
+      <c r="BC2" s="22"/>
+      <c r="BD2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="BE2" s="23"/>
-      <c r="BF2" s="23"/>
-      <c r="BG2" s="23" t="s">
+      <c r="BE2" s="22"/>
+      <c r="BF2" s="22"/>
+      <c r="BG2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="BH2" s="23"/>
-      <c r="BI2" s="23"/>
-      <c r="BJ2" s="24" t="s">
+      <c r="BH2" s="22"/>
+      <c r="BI2" s="22"/>
+      <c r="BJ2" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="BK2" s="24"/>
-      <c r="BL2" s="24"/>
-      <c r="BM2" s="24" t="s">
+      <c r="BK2" s="23"/>
+      <c r="BL2" s="23"/>
+      <c r="BM2" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="BN2" s="24"/>
-      <c r="BO2" s="24"/>
+      <c r="BN2" s="23"/>
+      <c r="BO2" s="23"/>
     </row>
     <row r="3" spans="1:67" ht="30" customHeight="1">
       <c r="A3">
@@ -65434,22 +65434,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AK2:AM2"/>
-    <mergeCell ref="AN2:AP2"/>
-    <mergeCell ref="AQ2:AS2"/>
-    <mergeCell ref="AT2:AV2"/>
-    <mergeCell ref="AW2:AY2"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="S1:AE1"/>
+    <mergeCell ref="AG1:AI1"/>
+    <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="AK1:AY1"/>
     <mergeCell ref="BA1:BO1"/>
     <mergeCell ref="BA2:BC2"/>
     <mergeCell ref="BD2:BF2"/>
     <mergeCell ref="BG2:BI2"/>
     <mergeCell ref="BJ2:BL2"/>
     <mergeCell ref="BM2:BO2"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="S1:AE1"/>
-    <mergeCell ref="AG1:AI1"/>
-    <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="AK1:AY1"/>
+    <mergeCell ref="AK2:AM2"/>
+    <mergeCell ref="AN2:AP2"/>
+    <mergeCell ref="AQ2:AS2"/>
+    <mergeCell ref="AT2:AV2"/>
+    <mergeCell ref="AW2:AY2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>